<commit_message>
(ver 1.0) Final Power Plant Project
</commit_message>
<xml_diff>
--- a/Sensitivity Spider Plots.xlsx
+++ b/Sensitivity Spider Plots.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="9555" windowHeight="9795"/>
+    <workbookView xWindow="28820" yWindow="1140" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Firing Temperature Sensitivity" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -637,34 +642,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2050</c:v>
+                  <c:v>2050.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2100</c:v>
+                  <c:v>2100.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2150</c:v>
+                  <c:v>2150.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2200</c:v>
+                  <c:v>2200.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2250</c:v>
+                  <c:v>2250.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2300</c:v>
+                  <c:v>2300.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2350</c:v>
+                  <c:v>2350.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2400</c:v>
+                  <c:v>2400.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2450</c:v>
+                  <c:v>2450.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2500</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,34 +681,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-1.0291647579783174</c:v>
+                  <c:v>-1.029164757978317</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.6871278057718736</c:v>
+                  <c:v>-0.687127805771873</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.34509085356542984</c:v>
+                  <c:v>-0.34509085356543</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34509085356542984</c:v>
+                  <c:v>0.34509085356543</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6871278057718736</c:v>
+                  <c:v>0.687127805771873</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0352725606962896</c:v>
+                  <c:v>1.03527256069629</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3834173156207055</c:v>
+                  <c:v>1.383417315620705</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7224003664681631</c:v>
+                  <c:v>1.722400366468163</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0674912200335926</c:v>
+                  <c:v>2.067491220033592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,34 +728,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2050</c:v>
+                  <c:v>2050.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2100</c:v>
+                  <c:v>2100.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2150</c:v>
+                  <c:v>2150.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2200</c:v>
+                  <c:v>2200.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2250</c:v>
+                  <c:v>2250.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2300</c:v>
+                  <c:v>2300.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2350</c:v>
+                  <c:v>2350.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2400</c:v>
+                  <c:v>2400.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2450</c:v>
+                  <c:v>2450.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2500</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,34 +767,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-12.656713955790158</c:v>
+                  <c:v>-12.65671395579016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8.4543055097327464</c:v>
+                  <c:v>-8.454305509732746</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.2354008578027065</c:v>
+                  <c:v>-4.235400857802706</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2518970636753535</c:v>
+                  <c:v>4.251897063675353</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.5120422302870491</c:v>
+                  <c:v>8.51204223028705</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.792807654239526</c:v>
+                  <c:v>12.79280765423953</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.081821181128344</c:v>
+                  <c:v>17.08182118112834</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.379082810953491</c:v>
+                  <c:v>21.37908281095349</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.696964698119434</c:v>
+                  <c:v>25.69696469811943</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,34 +814,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2050</c:v>
+                  <c:v>2050.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2100</c:v>
+                  <c:v>2100.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2150</c:v>
+                  <c:v>2150.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2200</c:v>
+                  <c:v>2200.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2250</c:v>
+                  <c:v>2250.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2300</c:v>
+                  <c:v>2300.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2350</c:v>
+                  <c:v>2350.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2400</c:v>
+                  <c:v>2400.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2450</c:v>
+                  <c:v>2450.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2500</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -848,31 +853,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>14.491483262656654</c:v>
+                  <c:v>14.49148326265665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.2345597119234366</c:v>
+                  <c:v>9.234559711923437</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4230176968088939</c:v>
+                  <c:v>4.423017696808894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.0771362914880021</c:v>
+                  <c:v>-4.077136291488002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-7.8439269384757466</c:v>
+                  <c:v>-7.843926938475747</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-11.340645803226639</c:v>
+                  <c:v>-11.34064580322664</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-14.588614342233061</c:v>
+                  <c:v>-14.58861434223306</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-17.613892113430143</c:v>
+                  <c:v>-17.61389211343014</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>-20.44253867475302</c:v>
@@ -890,15 +895,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="57434880"/>
-        <c:axId val="86983040"/>
+        <c:axId val="681966792"/>
+        <c:axId val="682354808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57434880"/>
+        <c:axId val="681966792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2500"/>
-          <c:min val="2000"/>
+          <c:max val="2500.0"/>
+          <c:min val="2000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -925,12 +930,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86983040"/>
+        <c:crossAx val="682354808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86983040"/>
+        <c:axId val="682354808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57434880"/>
+        <c:crossAx val="681966792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1029,78 +1034,48 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$14:$B$23</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$G$14:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>7.627089554800388</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>3.813544777400184</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>-3.813544777400204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>-7.63052208835342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$G$14:$G$23</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$H$14:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.11604825164147198</c:v>
+                  <c:v>30.12099085779802</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.718582989769431E-2</c:v>
+                  <c:v>23.42274386748333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3592914948847155E-2</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2215605435944419E-2</c:v>
+                  <c:v>-4.788341429562803</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.0539013589861047E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.7485112230874943E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.3293632615666515E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.1404794625133608</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.22904260192395787</c:v>
+                  <c:v>-9.89047461002323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1113,80 +1088,55 @@
           <c:tx>
             <c:v>Heat Rate</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$14:$B$23</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$G$14:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>7.627089554800388</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>3.813544777400184</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>-3.813544777400204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>-7.63052208835342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$H$14:$H$23</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$I$14:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.0438799076212586</c:v>
+                  <c:v>-10.73596980636693</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3942593203563289</c:v>
+                  <c:v>-12.43436166721366</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.699274166941608</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9135598812273269</c:v>
+                  <c:v>-2.86347226780441</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-2.0867700428901252</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-4.4127350709336755</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-7.0603761134938878</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-10.153414714615639</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-13.856812933025401</c:v>
+                  <c:v>-6.678700361010841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1201,78 +1151,48 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$14:$B$23</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$G$14:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>7.627089554800388</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>3.813544777400184</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>-3.813544777400204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>-7.63052208835342</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$I$14:$I$23</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$J$14:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-6.5788538532609895</c:v>
+                  <c:v>16.04920653042585</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.1195186088934079</c:v>
+                  <c:v>16.44879552460327</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.5654213356707984</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.8762881713297441</c:v>
+                  <c:v>0.468089964607825</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.1321456492383524</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.6172798559617183</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.5975456634526513</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.30274099168464</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.090592499585423</c:v>
+                  <c:v>0.94474255051946</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,11 +1207,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="57889536"/>
-        <c:axId val="57883648"/>
+        <c:axId val="575649528"/>
+        <c:axId val="609293288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57889536"/>
+        <c:axId val="575649528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,12 +1248,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57883648"/>
+        <c:crossAx val="609293288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57883648"/>
+        <c:axId val="609293288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,7 +1283,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57889536"/>
+        <c:crossAx val="575649528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1432,7 +1352,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$26:$B$36</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$23:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1474,42 +1394,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$G$26:$G$36</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$G$25:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-0.18323408153916629</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.1404794625133608</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.10383264620552755</c:v>
+                  <c:v>1.21545274087647</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-6.718582989769431E-2</c:v>
+                  <c:v>-0.0671858298976943</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.3592914948847155E-2</c:v>
+                  <c:v>-0.0335929149488471</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7485112230874943E-2</c:v>
+                  <c:v>0.0274851122308749</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.1078027179722091E-2</c:v>
+                  <c:v>0.0610780271797221</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.8563139410597042E-2</c:v>
+                  <c:v>0.088563139410597</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11910215300045808</c:v>
+                  <c:v>0.119102153000458</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1524,7 +1444,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$26:$B$35</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$23:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1563,39 +1483,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$H$26:$H$35</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$H$25:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-4.1941603431210694</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.266248762784548</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.3837017485978165</c:v>
+                  <c:v>0.527878587924792</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.5506433520290275</c:v>
+                  <c:v>-1.550643352029027</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.75470141867370433</c:v>
+                  <c:v>-0.754701418673704</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7175849554602568</c:v>
+                  <c:v>0.717584955460257</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4063015506433529</c:v>
+                  <c:v>1.406301550643353</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0620257340811725</c:v>
+                  <c:v>2.062025734081173</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6930056087100027</c:v>
+                  <c:v>2.693005608710003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1610,7 +1530,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$26:$B$35</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$23:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1649,39 +1569,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$I$26:$I$35</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$I$25:$I$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4.3803747838241227</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3758972779607306</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4448603444599737</c:v>
+                  <c:v>-16.9979389258724</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5730496789936357</c:v>
+                  <c:v>1.573049678993636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76283433228305442</c:v>
+                  <c:v>0.762834332283054</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.7130842671341624</c:v>
+                  <c:v>-0.713084267134162</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.3882637227262982</c:v>
+                  <c:v>-1.388263722726298</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.0208002653336767</c:v>
+                  <c:v>-2.020800265333677</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.6201700978417852</c:v>
+                  <c:v>-2.620170097841785</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1696,15 +1616,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81177984"/>
-        <c:axId val="81176448"/>
+        <c:axId val="582725000"/>
+        <c:axId val="582726424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81177984"/>
+        <c:axId val="582725000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0.70000000000000007"/>
+          <c:max val="1.0"/>
+          <c:min val="0.7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1731,12 +1651,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81176448"/>
+        <c:crossAx val="582726424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81176448"/>
+        <c:axId val="582726424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1766,7 +1686,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81177984"/>
+        <c:crossAx val="582725000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1818,7 +1738,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1835,7 +1754,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$38:$B$48</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$35:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1877,39 +1796,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$G$38:$G$47</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$G$37:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-0.21988089784699955</c:v>
+                  <c:v>-0.219880897847</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.17407237746220799</c:v>
+                  <c:v>-0.174072377462208</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.1252099557184303</c:v>
+                  <c:v>-0.12520995571843</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.2455336692624823E-2</c:v>
+                  <c:v>-0.0824553366926248</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.9700717666819367E-2</c:v>
+                  <c:v>-0.0397007176668194</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.9700717666819367E-2</c:v>
+                  <c:v>0.0397007176668194</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.3293632615666515E-2</c:v>
+                  <c:v>0.0732936326156665</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10688654756451366</c:v>
+                  <c:v>0.106886547564514</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1404794625133608</c:v>
+                  <c:v>0.140479462513361</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1924,7 +1843,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$38:$B$47</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$35:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1963,39 +1882,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$H$38:$H$47</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$H$37:$H$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-5.0973276146486191</c:v>
+                  <c:v>-5.09732761464862</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.9714615638403101</c:v>
+                  <c:v>-3.97146156384031</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.8992081821181142</c:v>
+                  <c:v>-2.899208182118114</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.8846915209501665</c:v>
+                  <c:v>-1.884691520950166</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.91966347740019738</c:v>
+                  <c:v>-0.919663477400197</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87842296271857867</c:v>
+                  <c:v>0.878422962718579</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7114813592873677</c:v>
+                  <c:v>1.711481359287368</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5115473441108618</c:v>
+                  <c:v>2.511547344110862</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2786209171890608</c:v>
+                  <c:v>3.278620917189061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2010,7 +1929,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$38:$B$47</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$35:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2049,39 +1968,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$I$38:$I$47</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$I$37:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.3706379853592718</c:v>
+                  <c:v>5.370637985359271</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1339935088010291</c:v>
+                  <c:v>4.13399350880103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9873729596550684</c:v>
+                  <c:v>2.987372959655068</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9213001350358927</c:v>
+                  <c:v>1.921300135035893</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9286678827793784</c:v>
+                  <c:v>0.928667882779378</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.86944161474497328</c:v>
+                  <c:v>-0.869441614744973</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-1.684395062898298</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.4495984459027174</c:v>
+                  <c:v>-2.449598445902717</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-3.1721589159223802</c:v>
+                  <c:v>-3.17215891592238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2096,15 +2015,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86643072"/>
-        <c:axId val="86583936"/>
+        <c:axId val="609762616"/>
+        <c:axId val="582029448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86643072"/>
+        <c:axId val="609762616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.95000000000000007"/>
-          <c:min val="0.70000000000000007"/>
+          <c:max val="0.95"/>
+          <c:min val="0.7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2124,19 +2043,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86583936"/>
+        <c:crossAx val="582029448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86583936"/>
+        <c:axId val="582029448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2159,21 +2077,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86643072"/>
+        <c:crossAx val="609762616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2232,10 +2148,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.3040011219971547E-2"/>
-          <c:y val="0.12486375566690526"/>
-          <c:w val="0.64895417843761893"/>
-          <c:h val="0.82331042710570257"/>
+          <c:x val="0.0930400112199715"/>
+          <c:y val="0.124863755666905"/>
+          <c:w val="0.648954178437619"/>
+          <c:h val="0.823310427105703"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2249,7 +2165,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$50:$B$59</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$47:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2281,46 +2197,46 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$G$50:$G$59</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$G$49:$G$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-0.15269506794930524</c:v>
+                  <c:v>-0.152695067949305</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.11604825164147198</c:v>
+                  <c:v>-0.116048251641472</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.8563139410597042E-2</c:v>
+                  <c:v>-0.088563139410597</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.8024125820735989E-2</c:v>
+                  <c:v>-0.058024125820736</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.0539013589861046E-2</c:v>
+                  <c:v>-0.030539013589861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0539013589861046E-2</c:v>
+                  <c:v>0.030539013589861</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.8024125820735989E-2</c:v>
+                  <c:v>0.058024125820736</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.2455336692624823E-2</c:v>
+                  <c:v>0.0824553366926248</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11299435028248588</c:v>
+                  <c:v>0.112994350282486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2335,7 +2251,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$50:$B$59</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$47:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2367,46 +2283,46 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$H$50:$H$59</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$H$49:$H$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.1836027713625936</c:v>
+                  <c:v>1.183602771362594</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95265588914551069</c:v>
+                  <c:v>0.952655889145511</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7175849554602568</c:v>
+                  <c:v>0.717584955460257</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47838997030683172</c:v>
+                  <c:v>0.478389970306832</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23919498515342502</c:v>
+                  <c:v>0.239194985153425</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.24331903662157772</c:v>
+                  <c:v>-0.243319036621578</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.48663807324315544</c:v>
+                  <c:v>-0.486638073243155</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.73408116133288592</c:v>
+                  <c:v>-0.734081161332886</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.98152424942263461</c:v>
+                  <c:v>-0.981524249422635</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2421,7 +2337,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$B$50:$B$59</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$B$47:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2453,46 +2369,46 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Firing Temperature Sensitivity'!$I$50:$I$59</c:f>
+              <c:f>'Firing Temperature Sensitivity'!$I$49:$I$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-1.1679420056383383</c:v>
+                  <c:v>-1.167942005638338</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.94288218710762206</c:v>
+                  <c:v>-0.942882187107622</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.71071521641278412</c:v>
+                  <c:v>-0.710715216412784</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.47617919499656769</c:v>
+                  <c:v>-0.476179194996568</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.23927412285897298</c:v>
+                  <c:v>-0.239274122858973</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24401222430172961</c:v>
+                  <c:v>0.24401222430173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.48802444860344607</c:v>
+                  <c:v>0.488024448603446</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.73914382506929754</c:v>
+                  <c:v>0.739143825069297</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99026320153514891</c:v>
+                  <c:v>0.990263201535149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2507,14 +2423,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81174912"/>
-        <c:axId val="81164544"/>
+        <c:axId val="609860808"/>
+        <c:axId val="582769624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81174912"/>
+        <c:axId val="609860808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2541,12 +2457,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81164544"/>
+        <c:crossAx val="582769624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81164544"/>
+        <c:axId val="582769624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2573,8 +2489,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="6.1068702290076335E-3"/>
-              <c:y val="0.29756430446194226"/>
+              <c:x val="0.00610687022900763"/>
+              <c:y val="0.297564304461942"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2583,7 +2499,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81174912"/>
+        <c:crossAx val="609860808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2609,15 +2525,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:colOff>568325</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2639,16 +2555,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2671,13 +2587,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2701,13 +2617,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2731,13 +2647,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3047,22 +2963,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3076,7 +2992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3105,7 +3021,7 @@
         <v>14.491483262656654</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="B3">
         <v>2100</v>
       </c>
@@ -3131,7 +3047,7 @@
         <v>9.2345597119234366</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="B4">
         <v>2150</v>
       </c>
@@ -3157,7 +3073,7 @@
         <v>4.4230176968088939</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="B5">
         <v>2200</v>
       </c>
@@ -3183,7 +3099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6">
         <v>2250</v>
       </c>
@@ -3209,7 +3125,7 @@
         <v>-4.0771362914880021</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="B7">
         <v>2300</v>
       </c>
@@ -3235,7 +3151,7 @@
         <v>-7.8439269384757466</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="B8">
         <v>2350</v>
       </c>
@@ -3261,7 +3177,7 @@
         <v>-11.340645803226639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9">
         <v>2400</v>
       </c>
@@ -3287,7 +3203,7 @@
         <v>-14.588614342233061</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="B10">
         <v>2450</v>
       </c>
@@ -3313,7 +3229,7 @@
         <v>-17.613892113430143</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="B11">
         <v>2500</v>
       </c>
@@ -3339,7 +3255,7 @@
         <v>-20.44253867475302</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3368,275 +3284,239 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14">
-        <v>25</v>
+        <v>269.11</v>
       </c>
       <c r="C14">
-        <v>32783</v>
+        <v>43126</v>
       </c>
       <c r="D14">
-        <v>2.5956000000000001</v>
+        <v>2.1758999999999999</v>
       </c>
       <c r="E14">
-        <v>0.39434000000000002</v>
+        <v>0.40659000000000001</v>
       </c>
       <c r="G14">
-        <f>(C14-$C$24) / ($C$24) *100</f>
-        <v>0.11604825164147198</v>
+        <f>($B$19 - B14) / $B$19 *100</f>
+        <v>7.6270895548003885</v>
       </c>
       <c r="H14">
-        <f>(D14-$D$24) / ($D$24) *100</f>
-        <v>7.0438799076212586</v>
+        <f>(C14- $C$19) / $C$19 *100</f>
+        <v>30.120990857798024</v>
       </c>
       <c r="I14">
-        <f>(E14-$E$24) / ($E$24) *100</f>
-        <v>-6.5788538532609895</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <f>(D14-$D$19)/$D$19 *100</f>
+        <v>-10.735969806366928</v>
+      </c>
+      <c r="J14">
+        <f>(E14-$E$19)/$E$19*100</f>
+        <v>16.049206530425845</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15">
-        <v>35</v>
+        <v>280.22000000000003</v>
       </c>
       <c r="C15">
-        <v>32767</v>
+        <v>40906</v>
       </c>
       <c r="D15">
-        <v>2.5556000000000001</v>
+        <v>2.1345000000000001</v>
       </c>
       <c r="E15">
-        <v>0.40050000000000002</v>
+        <v>0.40799000000000002</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15:G24" si="3">(C15-$C$24) / ($C$24) *100</f>
-        <v>6.718582989769431E-2</v>
+        <f t="shared" ref="G15:G19" si="3">($B$19 - B15) / $B$19 *100</f>
+        <v>3.8135447774001845</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H24" si="4">(D15-$D$24) / ($D$24) *100</f>
-        <v>5.3942593203563289</v>
+        <f t="shared" ref="H15:H19" si="4">(C15- $C$19) / $C$19 *100</f>
+        <v>23.42274386748333</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="I15:I24" si="5">(E15-$E$24) / ($E$24) *100</f>
-        <v>-5.1195186088934079</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I15:I19" si="5">(D15-$D$19)/$D$19 *100</f>
+        <v>-12.434361667213658</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ref="J15:J19" si="6">(E15-$E$19)/$E$19*100</f>
+        <v>16.44879552460327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="B16">
-        <v>45</v>
+        <v>291.33</v>
       </c>
       <c r="C16">
-        <v>32756</v>
+        <v>33143</v>
       </c>
       <c r="D16">
-        <v>2.5145</v>
+        <v>2.4376000000000002</v>
       </c>
       <c r="E16">
-        <v>0.40705999999999998</v>
+        <v>0.35036</v>
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>3.3592914948847155E-2</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <f t="shared" si="4"/>
-        <v>3.699274166941608</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <f t="shared" si="5"/>
-        <v>-3.5654213356707984</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="B17">
-        <v>55</v>
+        <v>302.44</v>
       </c>
       <c r="C17">
-        <v>32749</v>
+        <v>31556</v>
       </c>
       <c r="D17">
-        <v>2.4712000000000001</v>
+        <v>2.3677999999999999</v>
       </c>
       <c r="E17">
-        <v>0.41419</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>1.2215605435944419E-2</v>
+        <v>-3.813544777400204</v>
       </c>
       <c r="H17">
         <f t="shared" si="4"/>
-        <v>1.9135598812273269</v>
+        <v>-4.788341429562804</v>
       </c>
       <c r="I17">
         <f t="shared" si="5"/>
-        <v>-1.8762881713297441</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-2.86347226780441</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>0.46808996460782476</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="B18">
-        <v>65</v>
+        <v>313.56</v>
       </c>
       <c r="C18">
-        <v>32745</v>
+        <v>29865</v>
       </c>
       <c r="D18">
-        <v>2.4247999999999998</v>
+        <v>2.2747999999999999</v>
       </c>
       <c r="E18">
-        <v>0.42210999999999999</v>
+        <v>0.35366999999999998</v>
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-7.6305220883534197</v>
       </c>
       <c r="H18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-9.890474610023233</v>
       </c>
       <c r="I18">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-6.6787003610108409</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
+        <v>0.94474255051945988</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
       <c r="B19">
-        <v>75</v>
+        <f>B16</f>
+        <v>291.33</v>
       </c>
       <c r="C19">
-        <v>32746</v>
+        <f t="shared" ref="C19:E19" si="7">C16</f>
+        <v>33143</v>
       </c>
       <c r="D19">
-        <v>2.3742000000000001</v>
+        <f t="shared" si="7"/>
+        <v>2.4376000000000002</v>
       </c>
       <c r="E19">
-        <v>0.43110999999999999</v>
+        <f t="shared" si="7"/>
+        <v>0.35036</v>
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>3.0539013589861047E-3</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <f t="shared" si="4"/>
-        <v>-2.0867700428901252</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <f t="shared" si="5"/>
-        <v>2.1321456492383524</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>85</v>
-      </c>
-      <c r="C20">
-        <v>32754</v>
-      </c>
-      <c r="D20">
-        <v>2.3178000000000001</v>
-      </c>
-      <c r="E20">
-        <v>0.44159999999999999</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="3"/>
-        <v>2.7485112230874943E-2</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="4"/>
-        <v>-4.4127350709336755</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="5"/>
-        <v>4.6172798559617183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>95</v>
-      </c>
-      <c r="C21">
-        <v>32769</v>
-      </c>
-      <c r="D21">
-        <v>2.2536</v>
-      </c>
-      <c r="E21">
-        <v>0.45417999999999997</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="3"/>
-        <v>7.3293632615666515E-2</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="4"/>
-        <v>-7.0603761134938878</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="5"/>
-        <v>7.5975456634526513</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>105</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="C22">
-        <v>32791</v>
+        <v>32723</v>
       </c>
       <c r="D22">
-        <v>2.1785999999999999</v>
+        <v>2.3872</v>
       </c>
       <c r="E22">
-        <v>0.46982000000000002</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="3"/>
-        <v>0.1404794625133608</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="4"/>
-        <v>-10.153414714615639</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="5"/>
-        <v>11.30274099168464</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.42875000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
       <c r="B23">
-        <v>115</v>
+        <v>0.74</v>
       </c>
       <c r="C23">
-        <v>32820</v>
+        <v>32734</v>
       </c>
       <c r="D23">
-        <v>2.0888</v>
+        <v>2.4064999999999999</v>
       </c>
       <c r="E23">
-        <v>0.49003000000000002</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="3"/>
-        <v>0.22904260192395787</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="4"/>
-        <v>-13.856812933025401</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="5"/>
-        <v>16.090592499585423</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
+        <v>0.42532999999999999</v>
+      </c>
+      <c r="G23" t="e">
+        <f>(#REF!-#REF!) / (#REF!) *100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H23" t="e">
+        <f>(#REF!-#REF!) / (#REF!) *100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I23" t="e">
+        <f>(#REF!-#REF!) / (#REF!) *100</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="B24">
-        <v>65</v>
+        <v>0.76</v>
       </c>
       <c r="C24">
         <v>32745</v>
@@ -3647,898 +3527,832 @@
       <c r="E24">
         <v>0.42210999999999999</v>
       </c>
-      <c r="G24">
-        <f t="shared" si="3"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="B25">
+        <v>0.78</v>
+      </c>
+      <c r="C25">
+        <v>32754</v>
+      </c>
+      <c r="D25">
+        <v>2.4422000000000001</v>
+      </c>
+      <c r="E25">
+        <v>0.41909999999999997</v>
+      </c>
+      <c r="G25" t="e">
+        <f xml:space="preserve"> (#REF!-$C$29) / $C$29 *100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H25" t="e">
+        <f xml:space="preserve"> (#REF!-$D$29) / $D$29 *100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I25" t="e">
+        <f xml:space="preserve"> (#REF!-$E$29) / $E$29 *100</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="B26">
+        <v>0.8</v>
+      </c>
+      <c r="C26">
+        <v>32765</v>
+      </c>
+      <c r="D26">
+        <v>2.4588999999999999</v>
+      </c>
+      <c r="E26">
+        <v>0.41625000000000001</v>
+      </c>
+      <c r="G26" t="e">
+        <f xml:space="preserve"> (#REF!-$C$29) / $C$29 *100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H26" t="e">
+        <f xml:space="preserve"> (#REF!-$D$29) / $D$29 *100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I26" t="e">
+        <f xml:space="preserve"> (#REF!-$E$29) / $E$29 *100</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="B27">
+        <v>0.82</v>
+      </c>
+      <c r="C27">
+        <v>32774</v>
+      </c>
+      <c r="D27">
+        <v>2.4748000000000001</v>
+      </c>
+      <c r="E27">
+        <v>0.41358</v>
+      </c>
+      <c r="G27">
+        <f xml:space="preserve"> (C19-$C$29) / $C$29 *100</f>
+        <v>1.2154527408764697</v>
+      </c>
+      <c r="H27">
+        <f xml:space="preserve"> (D19-$D$29) / $D$29 *100</f>
+        <v>0.52787858792479248</v>
+      </c>
+      <c r="I27">
+        <f xml:space="preserve"> (E19-$E$29) / $E$29 *100</f>
+        <v>-16.997938925872401</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="B28">
+        <v>0.84</v>
+      </c>
+      <c r="C28">
+        <v>32784</v>
+      </c>
+      <c r="D28">
+        <v>2.4901</v>
+      </c>
+      <c r="E28">
+        <v>0.41105000000000003</v>
+      </c>
+      <c r="G28">
+        <f xml:space="preserve"> (C22-$C$29) / $C$29 *100</f>
+        <v>-6.718582989769431E-2</v>
+      </c>
+      <c r="H28">
+        <f xml:space="preserve"> (D22-$D$29) / $D$29 *100</f>
+        <v>-1.5506433520290275</v>
+      </c>
+      <c r="I28">
+        <f xml:space="preserve"> (E22-$E$29) / $E$29 *100</f>
+        <v>1.5730496789936357</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="B29">
+        <v>0.86</v>
+      </c>
+      <c r="C29">
+        <v>32745</v>
+      </c>
+      <c r="D29">
+        <v>2.4247999999999998</v>
+      </c>
+      <c r="E29">
+        <v>0.42210999999999999</v>
+      </c>
+      <c r="G29">
+        <f xml:space="preserve"> (C23-$C$29) / $C$29 *100</f>
+        <v>-3.3592914948847155E-2</v>
+      </c>
+      <c r="H29">
+        <f xml:space="preserve"> (D23-$D$29) / $D$29 *100</f>
+        <v>-0.75470141867370433</v>
+      </c>
+      <c r="I29">
+        <f xml:space="preserve"> (E23-$E$29) / $E$29 *100</f>
+        <v>0.76283433228305442</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30">
+        <v>0.88</v>
+      </c>
+      <c r="G30">
+        <f xml:space="preserve"> (C24-$C$29) / $C$29 *100</f>
         <v>0</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="4"/>
+      <c r="H30">
+        <f xml:space="preserve"> (D24-$D$29) / $D$29 *100</f>
         <v>0</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="5"/>
+      <c r="I30">
+        <f xml:space="preserve"> (E24-$E$29) / $E$29 *100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26">
+    <row r="31" spans="1:10">
+      <c r="B31">
+        <v>0.9</v>
+      </c>
+      <c r="C31">
+        <v>32673</v>
+      </c>
+      <c r="D31">
+        <v>2.3012000000000001</v>
+      </c>
+      <c r="E31">
+        <v>0.44478000000000001</v>
+      </c>
+      <c r="G31">
+        <f xml:space="preserve"> (C25-$C$29) / $C$29 *100</f>
+        <v>2.7485112230874943E-2</v>
+      </c>
+      <c r="H31">
+        <f xml:space="preserve"> (D25-$D$29) / $D$29 *100</f>
+        <v>0.7175849554602568</v>
+      </c>
+      <c r="I31">
+        <f xml:space="preserve"> (E25-$E$29) / $E$29 *100</f>
+        <v>-0.7130842671341624</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="B32">
+        <v>0.92</v>
+      </c>
+      <c r="C32">
+        <v>32688</v>
+      </c>
+      <c r="D32">
+        <v>2.3285</v>
+      </c>
+      <c r="E32">
+        <v>0.43956000000000001</v>
+      </c>
+      <c r="G32">
+        <f xml:space="preserve"> (C26-$C$29) / $C$29 *100</f>
+        <v>6.1078027179722091E-2</v>
+      </c>
+      <c r="H32">
+        <f xml:space="preserve"> (D26-$D$29) / $D$29 *100</f>
+        <v>1.4063015506433529</v>
+      </c>
+      <c r="I32">
+        <f xml:space="preserve"> (E26-$E$29) / $E$29 *100</f>
+        <v>-1.3882637227262982</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>0.84</v>
+      </c>
+      <c r="C33">
+        <v>32704</v>
+      </c>
+      <c r="D33">
+        <v>2.3544999999999998</v>
+      </c>
+      <c r="E33">
+        <v>0.43472</v>
+      </c>
+      <c r="G33">
+        <f xml:space="preserve"> (C27-$C$29) / $C$29 *100</f>
+        <v>8.8563139410597042E-2</v>
+      </c>
+      <c r="H33">
+        <f xml:space="preserve"> (D27-$D$29) / $D$29 *100</f>
+        <v>2.0620257340811725</v>
+      </c>
+      <c r="I33">
+        <f xml:space="preserve"> (E27-$E$29) / $E$29 *100</f>
+        <v>-2.0208002653336767</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="C34">
+        <v>32718</v>
+      </c>
+      <c r="D34">
+        <v>2.3791000000000002</v>
+      </c>
+      <c r="E34">
+        <v>0.43021999999999999</v>
+      </c>
+      <c r="G34">
+        <f xml:space="preserve"> (C28-$C$29) / $C$29 *100</f>
+        <v>0.11910215300045808</v>
+      </c>
+      <c r="H34">
+        <f xml:space="preserve"> (D28-$D$29) / $D$29 *100</f>
+        <v>2.6930056087100027</v>
+      </c>
+      <c r="I34">
+        <f xml:space="preserve"> (E28-$E$29) / $E$29 *100</f>
+        <v>-2.6201700978417852</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>0.72</v>
+      </c>
+      <c r="C35">
+        <v>32732</v>
+      </c>
+      <c r="D35">
+        <v>2.4024999999999999</v>
+      </c>
+      <c r="E35">
+        <v>0.42603000000000002</v>
+      </c>
+      <c r="G35">
+        <f xml:space="preserve"> (C29-$C$29) / $C$29 *100</f>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f xml:space="preserve"> (D29-$D$29) / $D$29 *100</f>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f xml:space="preserve"> (E29-$E$29) / $E$29 *100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="B36">
         <v>0.74</v>
       </c>
-      <c r="C26">
-        <v>32685</v>
-      </c>
-      <c r="D26">
-        <v>2.3231000000000002</v>
-      </c>
-      <c r="E26">
-        <v>0.44059999999999999</v>
-      </c>
-      <c r="G26">
-        <f xml:space="preserve"> (C26-$C$36) / $C$36 *100</f>
-        <v>-0.18323408153916629</v>
-      </c>
-      <c r="H26">
-        <f xml:space="preserve"> (D26-$D$36) / $D$36 *100</f>
-        <v>-4.1941603431210694</v>
-      </c>
-      <c r="I26">
-        <f xml:space="preserve"> (E26-$E$36) / $E$36 *100</f>
-        <v>4.3803747838241227</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="C36">
+        <v>32745</v>
+      </c>
+      <c r="D36">
+        <v>2.4247999999999998</v>
+      </c>
+      <c r="E36">
+        <v>0.42210999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="B37">
         <v>0.76</v>
       </c>
-      <c r="C27">
-        <v>32699</v>
-      </c>
-      <c r="D27">
-        <v>2.3456000000000001</v>
-      </c>
-      <c r="E27">
-        <v>0.43636000000000003</v>
-      </c>
-      <c r="G27">
-        <f t="shared" ref="G27:G36" si="6" xml:space="preserve"> (C27-$C$36) / $C$36 *100</f>
-        <v>-0.1404794625133608</v>
-      </c>
-      <c r="H27">
-        <f t="shared" ref="H27:H36" si="7" xml:space="preserve"> (D27-$D$36) / $D$36 *100</f>
-        <v>-3.266248762784548</v>
-      </c>
-      <c r="I27">
-        <f t="shared" ref="I27:I35" si="8" xml:space="preserve"> (E27-$E$36) / $E$36 *100</f>
-        <v>3.3758972779607306</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="C37">
+        <v>32758</v>
+      </c>
+      <c r="D37">
+        <v>2.4460999999999999</v>
+      </c>
+      <c r="E37">
+        <v>0.41843999999999998</v>
+      </c>
+      <c r="G37">
+        <f xml:space="preserve"> (C31-$C$41) / $C$41 *100</f>
+        <v>-0.21988089784699955</v>
+      </c>
+      <c r="H37">
+        <f xml:space="preserve"> (D31-$D$41) / $D$41 *100</f>
+        <v>-5.0973276146486191</v>
+      </c>
+      <c r="I37">
+        <f xml:space="preserve"> (E31-$E$41) / $E$41 *100</f>
+        <v>5.3706379853592718</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="B38">
         <v>0.78</v>
       </c>
-      <c r="C28">
-        <v>32711</v>
-      </c>
-      <c r="D28">
-        <v>2.367</v>
-      </c>
-      <c r="E28">
-        <v>0.43242999999999998</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="6"/>
-        <v>-0.10383264620552755</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="7"/>
-        <v>-2.3837017485978165</v>
-      </c>
-      <c r="I28">
+      <c r="C38">
+        <v>32769</v>
+      </c>
+      <c r="D38">
+        <v>2.4662999999999999</v>
+      </c>
+      <c r="E38">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:G47" si="8" xml:space="preserve"> (C32-$C$41) / $C$41 *100</f>
+        <v>-0.17407237746220799</v>
+      </c>
+      <c r="H38">
+        <f t="shared" ref="H38:H47" si="9" xml:space="preserve"> (D32-$D$41) / $D$41 *100</f>
+        <v>-3.9714615638403101</v>
+      </c>
+      <c r="I38">
+        <f t="shared" ref="I38:I47" si="10" xml:space="preserve"> (E32-$E$41) / $E$41 *100</f>
+        <v>4.1339935088010291</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="B39">
+        <v>0.8</v>
+      </c>
+      <c r="C39">
+        <v>32780</v>
+      </c>
+      <c r="D39">
+        <v>2.4857</v>
+      </c>
+      <c r="E39">
+        <v>0.41177000000000002</v>
+      </c>
+      <c r="G39">
         <f t="shared" si="8"/>
-        <v>2.4448603444599737</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>0.8</v>
-      </c>
-      <c r="C29">
-        <v>32723</v>
-      </c>
-      <c r="D29">
-        <v>2.3872</v>
-      </c>
-      <c r="E29">
-        <v>0.42875000000000002</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="6"/>
-        <v>-6.718582989769431E-2</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="7"/>
-        <v>-1.5506433520290275</v>
-      </c>
-      <c r="I29">
+        <v>-0.1252099557184303</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="9"/>
+        <v>-2.8992081821181142</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="10"/>
+        <v>2.9873729596550684</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="B40">
+        <v>0.82</v>
+      </c>
+      <c r="C40">
+        <v>32791</v>
+      </c>
+      <c r="D40">
+        <v>2.5043000000000002</v>
+      </c>
+      <c r="E40">
+        <v>0.40872000000000003</v>
+      </c>
+      <c r="G40">
         <f t="shared" si="8"/>
-        <v>1.5730496789936357</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>0.82</v>
-      </c>
-      <c r="C30">
-        <v>32734</v>
-      </c>
-      <c r="D30">
-        <v>2.4064999999999999</v>
-      </c>
-      <c r="E30">
-        <v>0.42532999999999999</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="6"/>
-        <v>-3.3592914948847155E-2</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="7"/>
-        <v>-0.75470141867370433</v>
-      </c>
-      <c r="I30">
+        <v>-8.2455336692624823E-2</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="9"/>
+        <v>-1.8846915209501665</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="10"/>
+        <v>1.9213001350358927</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="B41">
+        <v>0.84</v>
+      </c>
+      <c r="C41">
+        <v>32745</v>
+      </c>
+      <c r="D41">
+        <v>2.4247999999999998</v>
+      </c>
+      <c r="E41">
+        <v>0.42210999999999999</v>
+      </c>
+      <c r="G41">
         <f t="shared" si="8"/>
-        <v>0.76283433228305442</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>0.84</v>
-      </c>
-      <c r="C31">
-        <v>32745</v>
-      </c>
-      <c r="D31">
-        <v>2.4247999999999998</v>
-      </c>
-      <c r="E31">
-        <v>0.42210999999999999</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I31">
+        <v>-3.9700717666819367E-2</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="9"/>
+        <v>-0.91966347740019738</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="10"/>
+        <v>0.9286678827793784</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="B42">
+        <v>0.86</v>
+      </c>
+      <c r="G42">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>0.86</v>
-      </c>
-      <c r="C32">
-        <v>32754</v>
-      </c>
-      <c r="D32">
-        <v>2.4422000000000001</v>
-      </c>
-      <c r="E32">
-        <v>0.41909999999999997</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="6"/>
-        <v>2.7485112230874943E-2</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="7"/>
-        <v>0.7175849554602568</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="8"/>
-        <v>-0.7130842671341624</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>0.88</v>
-      </c>
-      <c r="C33">
-        <v>32765</v>
-      </c>
-      <c r="D33">
-        <v>2.4588999999999999</v>
-      </c>
-      <c r="E33">
-        <v>0.41625000000000001</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="6"/>
-        <v>6.1078027179722091E-2</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="7"/>
-        <v>1.4063015506433529</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="8"/>
-        <v>-1.3882637227262982</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>0.9</v>
-      </c>
-      <c r="C34">
-        <v>32774</v>
-      </c>
-      <c r="D34">
-        <v>2.4748000000000001</v>
-      </c>
-      <c r="E34">
-        <v>0.41358</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="6"/>
-        <v>8.8563139410597042E-2</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="7"/>
-        <v>2.0620257340811725</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="8"/>
-        <v>-2.0208002653336767</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>0.92</v>
-      </c>
-      <c r="C35">
-        <v>32784</v>
-      </c>
-      <c r="D35">
-        <v>2.4901</v>
-      </c>
-      <c r="E35">
-        <v>0.41105000000000003</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="6"/>
-        <v>0.11910215300045808</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="7"/>
-        <v>2.6930056087100027</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="8"/>
-        <v>-2.6201700978417852</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36">
-        <v>0.84</v>
-      </c>
-      <c r="C36">
-        <v>32745</v>
-      </c>
-      <c r="D36">
-        <v>2.4247999999999998</v>
-      </c>
-      <c r="E36">
-        <v>0.42210999999999999</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <f xml:space="preserve"> (E36-$E$36) / $E$36 *100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38">
-        <v>0.72</v>
-      </c>
-      <c r="C38">
-        <v>32673</v>
-      </c>
-      <c r="D38">
-        <v>2.3012000000000001</v>
-      </c>
-      <c r="E38">
-        <v>0.44478000000000001</v>
-      </c>
-      <c r="G38">
-        <f xml:space="preserve"> (C38-$C$48) / $C$48 *100</f>
-        <v>-0.21988089784699955</v>
-      </c>
-      <c r="H38">
-        <f xml:space="preserve"> (D38-$D$48) / $D$48 *100</f>
-        <v>-5.0973276146486191</v>
-      </c>
-      <c r="I38">
-        <f xml:space="preserve"> (E38-$E$48) / $E$48 *100</f>
-        <v>5.3706379853592718</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>0.74</v>
-      </c>
-      <c r="C39">
-        <v>32688</v>
-      </c>
-      <c r="D39">
-        <v>2.3285</v>
-      </c>
-      <c r="E39">
-        <v>0.43956000000000001</v>
-      </c>
-      <c r="G39">
-        <f t="shared" ref="G39:G48" si="9" xml:space="preserve"> (C39-$C$48) / $C$48 *100</f>
-        <v>-0.17407237746220799</v>
-      </c>
-      <c r="H39">
-        <f t="shared" ref="H39:H48" si="10" xml:space="preserve"> (D39-$D$48) / $D$48 *100</f>
-        <v>-3.9714615638403101</v>
-      </c>
-      <c r="I39">
-        <f t="shared" ref="I39:I48" si="11" xml:space="preserve"> (E39-$E$48) / $E$48 *100</f>
-        <v>4.1339935088010291</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>0.76</v>
-      </c>
-      <c r="C40">
-        <v>32704</v>
-      </c>
-      <c r="D40">
-        <v>2.3544999999999998</v>
-      </c>
-      <c r="E40">
-        <v>0.43472</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="9"/>
-        <v>-0.1252099557184303</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="10"/>
-        <v>-2.8992081821181142</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="11"/>
-        <v>2.9873729596550684</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>0.78</v>
-      </c>
-      <c r="C41">
-        <v>32718</v>
-      </c>
-      <c r="D41">
-        <v>2.3791000000000002</v>
-      </c>
-      <c r="E41">
-        <v>0.43021999999999999</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="9"/>
-        <v>-8.2455336692624823E-2</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="10"/>
-        <v>-1.8846915209501665</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="11"/>
-        <v>1.9213001350358927</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>0.8</v>
-      </c>
-      <c r="C42">
-        <v>32732</v>
-      </c>
-      <c r="D42">
-        <v>2.4024999999999999</v>
-      </c>
-      <c r="E42">
-        <v>0.42603000000000002</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="9"/>
-        <v>-3.9700717666819367E-2</v>
-      </c>
       <c r="H42">
-        <f t="shared" si="10"/>
-        <v>-0.91966347740019738</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="11"/>
-        <v>0.9286678827793784</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>0.82</v>
-      </c>
-      <c r="C43">
-        <v>32745</v>
-      </c>
-      <c r="D43">
-        <v>2.4247999999999998</v>
-      </c>
-      <c r="E43">
-        <v>0.42210999999999999</v>
-      </c>
-      <c r="G43">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H43">
+      <c r="I42">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="B43">
+        <v>0.88</v>
+      </c>
+      <c r="C43">
+        <v>32695</v>
+      </c>
+      <c r="D43">
+        <v>2.4535</v>
+      </c>
+      <c r="E43">
+        <v>0.41718</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="8"/>
+        <v>3.9700717666819367E-2</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="9"/>
+        <v>0.87842296271857867</v>
+      </c>
       <c r="I43">
+        <f t="shared" si="10"/>
+        <v>-0.86944161474497328</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="B44">
+        <v>0.9</v>
+      </c>
+      <c r="C44">
+        <v>32707</v>
+      </c>
+      <c r="D44">
+        <v>2.4479000000000002</v>
+      </c>
+      <c r="E44">
+        <v>0.41813</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="8"/>
+        <v>7.3293632615666515E-2</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="9"/>
+        <v>1.7114813592873677</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="10"/>
+        <v>-1.684395062898298</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45">
+        <v>0.82</v>
+      </c>
+      <c r="C45">
+        <v>32716</v>
+      </c>
+      <c r="D45">
+        <v>2.4422000000000001</v>
+      </c>
+      <c r="E45">
+        <v>0.41910999999999998</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="8"/>
+        <v>0.10688654756451366</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="9"/>
+        <v>2.5115473441108618</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="10"/>
+        <v>-2.4495984459027174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="C46">
+        <v>32726</v>
+      </c>
+      <c r="D46">
+        <v>2.4363999999999999</v>
+      </c>
+      <c r="E46">
+        <v>0.42009999999999997</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="8"/>
+        <v>0.1404794625133608</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="9"/>
+        <v>3.2786209171890608</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="10"/>
+        <v>-3.1721589159223802</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>0.1</v>
+      </c>
+      <c r="C47">
+        <v>32735</v>
+      </c>
+      <c r="D47">
+        <v>2.4306000000000001</v>
+      </c>
+      <c r="E47">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="B48">
+        <v>0.2</v>
+      </c>
+      <c r="C48">
+        <v>32745</v>
+      </c>
+      <c r="D48">
+        <v>2.4247999999999998</v>
+      </c>
+      <c r="E48">
+        <v>0.42210999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="B49">
+        <v>0.3</v>
+      </c>
+      <c r="C49">
+        <v>32755</v>
+      </c>
+      <c r="D49">
+        <v>2.4188999999999998</v>
+      </c>
+      <c r="E49">
+        <v>0.42314000000000002</v>
+      </c>
+      <c r="G49">
+        <f xml:space="preserve"> (C43-$C$53) / $C$53 *100</f>
+        <v>-0.15269506794930524</v>
+      </c>
+      <c r="H49">
+        <f xml:space="preserve"> (D43-$D$53) / $D$53 *100</f>
+        <v>1.1836027713625936</v>
+      </c>
+      <c r="I49">
+        <f xml:space="preserve"> (E43-$E$53) / $E$53 *100</f>
+        <v>-1.1679420056383383</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="B50">
+        <v>0.4</v>
+      </c>
+      <c r="C50">
+        <v>32764</v>
+      </c>
+      <c r="D50">
+        <v>2.4129999999999998</v>
+      </c>
+      <c r="E50">
+        <v>0.42416999999999999</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ref="G50:G59" si="11" xml:space="preserve"> (C44-$C$53) / $C$53 *100</f>
+        <v>-0.11604825164147198</v>
+      </c>
+      <c r="H50">
+        <f t="shared" ref="H50:H59" si="12" xml:space="preserve"> (D44-$D$53) / $D$53 *100</f>
+        <v>0.95265588914551069</v>
+      </c>
+      <c r="I50">
+        <f t="shared" ref="I50:I59" si="13" xml:space="preserve"> (E44-$E$53) / $E$53 *100</f>
+        <v>-0.94288218710762206</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="B51">
+        <v>0.5</v>
+      </c>
+      <c r="C51">
+        <v>32772</v>
+      </c>
+      <c r="D51">
+        <v>2.407</v>
+      </c>
+      <c r="E51">
+        <v>0.42523</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="11"/>
+        <v>-8.8563139410597042E-2</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="12"/>
+        <v>0.7175849554602568</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="13"/>
+        <v>-0.71071521641278412</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="B52">
+        <v>0.6</v>
+      </c>
+      <c r="C52">
+        <v>32782</v>
+      </c>
+      <c r="D52">
+        <v>2.4009999999999998</v>
+      </c>
+      <c r="E52">
+        <v>0.42629</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="11"/>
+        <v>-5.8024125820735989E-2</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="12"/>
+        <v>0.47838997030683172</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="13"/>
+        <v>-0.47617919499656769</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="B53">
+        <v>0.7</v>
+      </c>
+      <c r="C53">
+        <v>32745</v>
+      </c>
+      <c r="D53">
+        <v>2.4247999999999998</v>
+      </c>
+      <c r="E53">
+        <v>0.42210999999999999</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="11"/>
+        <v>-3.0539013589861046E-2</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="12"/>
+        <v>0.23919498515342502</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="13"/>
+        <v>-0.23927412285897298</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="B54">
+        <v>0.8</v>
+      </c>
+      <c r="G54">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>0.84</v>
-      </c>
-      <c r="C44">
-        <v>32758</v>
-      </c>
-      <c r="D44">
-        <v>2.4460999999999999</v>
-      </c>
-      <c r="E44">
-        <v>0.41843999999999998</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="9"/>
-        <v>3.9700717666819367E-2</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="10"/>
-        <v>0.87842296271857867</v>
-      </c>
-      <c r="I44">
+      <c r="H54">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="B55">
+        <v>0.9</v>
+      </c>
+      <c r="G55">
         <f t="shared" si="11"/>
-        <v>-0.86944161474497328</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>0.86</v>
-      </c>
-      <c r="C45">
-        <v>32769</v>
-      </c>
-      <c r="D45">
-        <v>2.4662999999999999</v>
-      </c>
-      <c r="E45">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="9"/>
-        <v>7.3293632615666515E-2</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="10"/>
-        <v>1.7114813592873677</v>
-      </c>
-      <c r="I45">
+        <v>3.0539013589861046E-2</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="12"/>
+        <v>-0.24331903662157772</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="13"/>
+        <v>0.24401222430172961</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="G56">
         <f t="shared" si="11"/>
-        <v>-1.684395062898298</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>0.88</v>
-      </c>
-      <c r="C46">
-        <v>32780</v>
-      </c>
-      <c r="D46">
-        <v>2.4857</v>
-      </c>
-      <c r="E46">
-        <v>0.41177000000000002</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="9"/>
-        <v>0.10688654756451366</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="10"/>
-        <v>2.5115473441108618</v>
-      </c>
-      <c r="I46">
+        <v>5.8024125820735989E-2</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="12"/>
+        <v>-0.48663807324315544</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="13"/>
+        <v>0.48802444860344607</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57">
+        <v>0.6</v>
+      </c>
+      <c r="G57">
         <f t="shared" si="11"/>
-        <v>-2.4495984459027174</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>0.9</v>
-      </c>
-      <c r="C47">
-        <v>32791</v>
-      </c>
-      <c r="D47">
-        <v>2.5043000000000002</v>
-      </c>
-      <c r="E47">
-        <v>0.40872000000000003</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="9"/>
-        <v>0.1404794625133608</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="10"/>
-        <v>3.2786209171890608</v>
-      </c>
-      <c r="I47">
+        <v>8.2455336692624823E-2</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="12"/>
+        <v>-0.73408116133288592</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="13"/>
+        <v>0.73914382506929754</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="G58">
         <f t="shared" si="11"/>
-        <v>-3.1721589159223802</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48">
-        <v>0.82</v>
-      </c>
-      <c r="C48">
-        <v>32745</v>
-      </c>
-      <c r="D48">
-        <v>2.4247999999999998</v>
-      </c>
-      <c r="E48">
-        <v>0.42210999999999999</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I48">
+        <v>0.11299435028248588</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="12"/>
+        <v>-0.98152424942263461</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="13"/>
+        <v>0.99026320153514891</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="G59">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50">
-        <v>0.1</v>
-      </c>
-      <c r="C50">
-        <v>32695</v>
-      </c>
-      <c r="D50">
-        <v>2.4535</v>
-      </c>
-      <c r="E50">
-        <v>0.41718</v>
-      </c>
-      <c r="G50">
-        <f xml:space="preserve"> (C50-$C$60) / $C$60 *100</f>
-        <v>-0.15269506794930524</v>
-      </c>
-      <c r="H50">
-        <f xml:space="preserve"> (D50-$D$60) / $D$60 *100</f>
-        <v>1.1836027713625936</v>
-      </c>
-      <c r="I50">
-        <f xml:space="preserve"> (E50-$E$60) / $E$60 *100</f>
-        <v>-1.1679420056383383</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>0.2</v>
-      </c>
-      <c r="C51">
-        <v>32707</v>
-      </c>
-      <c r="D51">
-        <v>2.4479000000000002</v>
-      </c>
-      <c r="E51">
-        <v>0.41813</v>
-      </c>
-      <c r="G51">
-        <f t="shared" ref="G51:G60" si="12" xml:space="preserve"> (C51-$C$60) / $C$60 *100</f>
-        <v>-0.11604825164147198</v>
-      </c>
-      <c r="H51">
-        <f t="shared" ref="H51:H60" si="13" xml:space="preserve"> (D51-$D$60) / $D$60 *100</f>
-        <v>0.95265588914551069</v>
-      </c>
-      <c r="I51">
-        <f t="shared" ref="I51:I60" si="14" xml:space="preserve"> (E51-$E$60) / $E$60 *100</f>
-        <v>-0.94288218710762206</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>0.3</v>
-      </c>
-      <c r="C52">
-        <v>32716</v>
-      </c>
-      <c r="D52">
-        <v>2.4422000000000001</v>
-      </c>
-      <c r="E52">
-        <v>0.41910999999999998</v>
-      </c>
-      <c r="G52">
-        <f t="shared" si="12"/>
-        <v>-8.8563139410597042E-2</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="13"/>
-        <v>0.7175849554602568</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="14"/>
-        <v>-0.71071521641278412</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B53">
-        <v>0.4</v>
-      </c>
-      <c r="C53">
-        <v>32726</v>
-      </c>
-      <c r="D53">
-        <v>2.4363999999999999</v>
-      </c>
-      <c r="E53">
-        <v>0.42009999999999997</v>
-      </c>
-      <c r="G53">
-        <f t="shared" si="12"/>
-        <v>-5.8024125820735989E-2</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="13"/>
-        <v>0.47838997030683172</v>
-      </c>
-      <c r="I53">
-        <f t="shared" si="14"/>
-        <v>-0.47617919499656769</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B54">
-        <v>0.5</v>
-      </c>
-      <c r="C54">
-        <v>32735</v>
-      </c>
-      <c r="D54">
-        <v>2.4306000000000001</v>
-      </c>
-      <c r="E54">
-        <v>0.42109999999999997</v>
-      </c>
-      <c r="G54">
-        <f t="shared" si="12"/>
-        <v>-3.0539013589861046E-2</v>
-      </c>
-      <c r="H54">
-        <f t="shared" si="13"/>
-        <v>0.23919498515342502</v>
-      </c>
-      <c r="I54">
-        <f t="shared" si="14"/>
-        <v>-0.23927412285897298</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B55">
-        <v>0.6</v>
-      </c>
-      <c r="C55">
-        <v>32745</v>
-      </c>
-      <c r="D55">
-        <v>2.4247999999999998</v>
-      </c>
-      <c r="E55">
-        <v>0.42210999999999999</v>
-      </c>
-      <c r="G55">
+      <c r="H59">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="H55">
+      <c r="I59">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="I55">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B56">
-        <v>0.7</v>
-      </c>
-      <c r="C56">
-        <v>32755</v>
-      </c>
-      <c r="D56">
-        <v>2.4188999999999998</v>
-      </c>
-      <c r="E56">
-        <v>0.42314000000000002</v>
-      </c>
-      <c r="G56">
-        <f t="shared" si="12"/>
-        <v>3.0539013589861046E-2</v>
-      </c>
-      <c r="H56">
-        <f t="shared" si="13"/>
-        <v>-0.24331903662157772</v>
-      </c>
-      <c r="I56">
-        <f t="shared" si="14"/>
-        <v>0.24401222430172961</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B57">
-        <v>0.8</v>
-      </c>
-      <c r="C57">
-        <v>32764</v>
-      </c>
-      <c r="D57">
-        <v>2.4129999999999998</v>
-      </c>
-      <c r="E57">
-        <v>0.42416999999999999</v>
-      </c>
-      <c r="G57">
-        <f t="shared" si="12"/>
-        <v>5.8024125820735989E-2</v>
-      </c>
-      <c r="H57">
-        <f t="shared" si="13"/>
-        <v>-0.48663807324315544</v>
-      </c>
-      <c r="I57">
-        <f t="shared" si="14"/>
-        <v>0.48802444860344607</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58">
-        <v>0.9</v>
-      </c>
-      <c r="C58">
-        <v>32772</v>
-      </c>
-      <c r="D58">
-        <v>2.407</v>
-      </c>
-      <c r="E58">
-        <v>0.42523</v>
-      </c>
-      <c r="G58">
-        <f t="shared" si="12"/>
-        <v>8.2455336692624823E-2</v>
-      </c>
-      <c r="H58">
-        <f t="shared" si="13"/>
-        <v>-0.73408116133288592</v>
-      </c>
-      <c r="I58">
-        <f t="shared" si="14"/>
-        <v>0.73914382506929754</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59">
-        <v>32782</v>
-      </c>
-      <c r="D59">
-        <v>2.4009999999999998</v>
-      </c>
-      <c r="E59">
-        <v>0.42629</v>
-      </c>
-      <c r="G59">
-        <f t="shared" si="12"/>
-        <v>0.11299435028248588</v>
-      </c>
-      <c r="H59">
-        <f t="shared" si="13"/>
-        <v>-0.98152424942263461</v>
-      </c>
-      <c r="I59">
-        <f t="shared" si="14"/>
-        <v>0.99026320153514891</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60">
-        <v>0.6</v>
-      </c>
-      <c r="C60">
-        <v>32745</v>
-      </c>
-      <c r="D60">
-        <v>2.4247999999999998</v>
-      </c>
-      <c r="E60">
-        <v>0.42210999999999999</v>
-      </c>
-      <c r="G60">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>